<commit_message>
start of tab 25
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_25_rpt_PA_LessonsLearnedbyCategory.xlsx
+++ b/backend/reports/xlsx/Tab_25_rpt_PA_LessonsLearnedbyCategory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aspiteri/Development/Github/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66A533A6-ED0D-7448-97F7-D4E319699D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5035F81F-5752-284D-9194-6BFE6500E1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36920" yWindow="-21100" windowWidth="21600" windowHeight="37900" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="12920" yWindow="12800" windowWidth="51200" windowHeight="26660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,30 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>{#r=d.report[i]}</t>
+    <t>Lessons Learned by Category</t>
   </si>
   <si>
-    <t>{#r1=d.report[i+1]}</t>
-  </si>
-  <si>
-    <t>{#t=d.report_totals[i]}</t>
-  </si>
-  <si>
-    <t>{#date=d.date}</t>
-  </si>
-  <si>
-    <t>Project #</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
-    <t>{#fy=d.fiscal_year}</t>
-  </si>
-  <si>
-    <t>Project ________ for {$fy} as of {$date}</t>
+    <t>Portfolio: {}</t>
   </si>
 </sst>
 </file>
@@ -69,7 +51,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,11 +64,6 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
       <sz val="8.5"/>
       <name val="BCSans-Regular"/>
     </font>
@@ -105,8 +82,18 @@
       <color theme="1"/>
       <name val="BCSans-Regular"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="BCSans-Regular"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,82 +106,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA5A5A5"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFA5A5A5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -205,45 +123,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="24"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="6"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -273,15 +181,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>312615</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1561691</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>680356</xdr:rowOff>
+      <xdr:colOff>1159482</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>185615</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -310,8 +218,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2411054" cy="680356"/>
+          <a:off x="312615" y="127000"/>
+          <a:ext cx="1696790" cy="478692"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -324,9 +232,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -364,7 +272,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -470,7 +378,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -612,7 +520,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -623,112 +531,155 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I2" sqref="C2:I2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
     <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="9" width="15.83203125" customWidth="1"/>
+    <col min="3" max="6" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="33" customHeight="1">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
       <c r="C1" s="16" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
+    </row>
+    <row r="2" spans="1:10" s="5" customFormat="1" ht="25" customHeight="1">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="15" t="s">
+        <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="19">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
       <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="19">
+      <c r="A4" s="7"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
       <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="19">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="14"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="14"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="14"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="14"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="14"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Add tab 25 report template fixes
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_25_rpt_PA_LessonsLearnedbyCategory.xlsx
+++ b/backend/reports/xlsx/Tab_25_rpt_PA_LessonsLearnedbyCategory.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aspiteri/Development/Github/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5035F81F-5752-284D-9194-6BFE6500E1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920C480C-BB8F-9142-B724-AE4924CF0061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12920" yWindow="12800" windowWidth="51200" windowHeight="26660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$3:$3</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,12 +39,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Lessons Learned by Category</t>
   </si>
   <si>
-    <t>Portfolio: {}</t>
+    <t>Lesson Sub Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lesson Learned </t>
+  </si>
+  <si>
+    <t>Recommendation</t>
+  </si>
+  <si>
+    <t>{$llcat}</t>
+  </si>
+  <si>
+    <t>{$llcat1}</t>
+  </si>
+  <si>
+    <t>{#llcat=d.reportLessonsLearned[i].category}</t>
+  </si>
+  <si>
+    <t>{#llcat1=d.reportLessonsLearned[i+1].category}</t>
+  </si>
+  <si>
+    <t>{$ll.project_number}</t>
+  </si>
+  <si>
+    <t>{$ll.project_name}</t>
+  </si>
+  <si>
+    <t>{$ll.portfolio_abbrev}</t>
+  </si>
+  <si>
+    <t>{$ll.lesson_sub_category}</t>
+  </si>
+  <si>
+    <t>{$ll.lesson}</t>
+  </si>
+  <si>
+    <t>{$ll.recommendations}</t>
+  </si>
+  <si>
+    <t>{#ll=d.reportLessonsLearned[i].info[i]}</t>
+  </si>
+  <si>
+    <t>{#ll1=d.reportLessonsLearned[i].info[i+1]}</t>
+  </si>
+  <si>
+    <t>{$ll1}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="0"/>
+        <rFont val="BC Sans Regular"/>
+      </rPr>
+      <t>Portfolios</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0"/>
+        <rFont val="BC Sans Regular"/>
+      </rPr>
+      <t>: {d.reportPortfolio.portfolioNames}</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -51,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -60,40 +130,72 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
       <sz val="12"/>
-      <name val="BCSans-Regular"/>
+      <name val="BC Sans Regular"/>
     </font>
     <font>
       <sz val="8.5"/>
-      <name val="BCSans-Regular"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF38B9C7"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="BC Sans Regular"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <color theme="0"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="0"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="BCSans-Regular"/>
+      <name val="BC Sans Regular"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,8 +208,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -115,43 +223,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="24"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="6"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -181,15 +353,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>312615</xdr:colOff>
+      <xdr:colOff>312614</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1159482</xdr:colOff>
+      <xdr:colOff>1990564</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>185615</xdr:rowOff>
+      <xdr:rowOff>420077</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -218,8 +390,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="312615" y="127000"/>
-          <a:ext cx="1696790" cy="478692"/>
+          <a:off x="312614" y="127000"/>
+          <a:ext cx="2527873" cy="713154"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -531,158 +703,143 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="6" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="43.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="39.1640625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" style="2" outlineLevel="1"/>
+    <col min="9" max="16383" width="10.83203125" style="2" customWidth="1"/>
+    <col min="16384" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="33" customHeight="1">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="16" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="33" customHeight="1">
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-    </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" ht="25" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="15" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="45" customHeight="1">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:8" s="5" customFormat="1" ht="17">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="19">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-    </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="19">
-      <c r="A4" s="7"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="19">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="14"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="14"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="14"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="14"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="14"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="3"/>
+      <c r="E3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1">
+      <c r="A4" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1">
+      <c r="A5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="G8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="H13" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="5" scale="68" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddFooter>&amp;LTab_43_rpt_PF_RecoveryForecast
 &amp;C&amp;P of &amp;N&amp;R{$date}</oddFooter>

</xml_diff>

<commit_message>
Bug/tab 25 rpt p lessons learned by category (#744)
* start of tab 25

* Add tab 25 report template fixes

* lint fixes

* fixed test

* lint
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_25_rpt_PA_LessonsLearnedbyCategory.xlsx
+++ b/backend/reports/xlsx/Tab_25_rpt_PA_LessonsLearnedbyCategory.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aspiteri/Development/Github/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66A533A6-ED0D-7448-97F7-D4E319699D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920C480C-BB8F-9142-B724-AE4924CF0061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36920" yWindow="-21100" windowWidth="21600" windowHeight="37900" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$3:$3</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,30 +39,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>{#r=d.report[i]}</t>
-  </si>
-  <si>
-    <t>{#r1=d.report[i+1]}</t>
-  </si>
-  <si>
-    <t>{#t=d.report_totals[i]}</t>
-  </si>
-  <si>
-    <t>{#date=d.date}</t>
-  </si>
-  <si>
-    <t>Project #</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
-    <t>{#fy=d.fiscal_year}</t>
-  </si>
-  <si>
-    <t>Project ________ for {$fy} as of {$date}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>Lessons Learned by Category</t>
+  </si>
+  <si>
+    <t>Lesson Sub Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lesson Learned </t>
+  </si>
+  <si>
+    <t>Recommendation</t>
+  </si>
+  <si>
+    <t>{$llcat}</t>
+  </si>
+  <si>
+    <t>{$llcat1}</t>
+  </si>
+  <si>
+    <t>{#llcat=d.reportLessonsLearned[i].category}</t>
+  </si>
+  <si>
+    <t>{#llcat1=d.reportLessonsLearned[i+1].category}</t>
+  </si>
+  <si>
+    <t>{$ll.project_number}</t>
+  </si>
+  <si>
+    <t>{$ll.project_name}</t>
+  </si>
+  <si>
+    <t>{$ll.portfolio_abbrev}</t>
+  </si>
+  <si>
+    <t>{$ll.lesson_sub_category}</t>
+  </si>
+  <si>
+    <t>{$ll.lesson}</t>
+  </si>
+  <si>
+    <t>{$ll.recommendations}</t>
+  </si>
+  <si>
+    <t>{#ll=d.reportLessonsLearned[i].info[i]}</t>
+  </si>
+  <si>
+    <t>{#ll1=d.reportLessonsLearned[i].info[i+1]}</t>
+  </si>
+  <si>
+    <t>{$ll1}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="0"/>
+        <rFont val="BC Sans Regular"/>
+      </rPr>
+      <t>Portfolios</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0"/>
+        <rFont val="BC Sans Regular"/>
+      </rPr>
+      <t>: {d.reportPortfolio.portfolioNames}</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -69,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -78,32 +130,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
       <sz val="12"/>
-      <name val="BCSans-Regular"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <sz val="8.5"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="BC Sans Regular"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <sz val="8.5"/>
-      <name val="BCSans-Regular"/>
+      <sz val="11"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="BC Sans Regular"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF38B9C7"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="BC Sans Regular"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <color theme="0"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="BCSans-Regular"/>
+      <name val="BC Sans Regular"/>
     </font>
   </fonts>
   <fills count="4">
@@ -126,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -135,65 +224,56 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
+      <left style="thin">
+        <color theme="0"/>
       </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
+      <right style="thin">
+        <color theme="0"/>
       </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
+      <top style="thin">
+        <color theme="0"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
+      <bottom style="thin">
+        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
+      <left style="thin">
+        <color theme="0"/>
       </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
+      <right style="thin">
+        <color theme="0"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
+      <left style="thin">
+        <color theme="0"/>
       </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
+      <right style="thin">
+        <color theme="0"/>
       </right>
-      <top style="medium">
-        <color rgb="FFA5A5A5"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFA5A5A5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
+      <top style="thin">
+        <color theme="0"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
+      <bottom style="thin">
+        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
@@ -201,49 +281,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -273,15 +353,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>312614</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1561691</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>680356</xdr:rowOff>
+      <xdr:colOff>1990564</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>420077</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -310,8 +390,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2411054" cy="680356"/>
+          <a:off x="312614" y="127000"/>
+          <a:ext cx="2527873" cy="713154"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -324,9 +404,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -364,7 +444,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -470,7 +550,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -612,7 +692,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -623,115 +703,143 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I2" sqref="C2:I2"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="9" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="43.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="39.1640625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" style="2" outlineLevel="1"/>
+    <col min="9" max="16383" width="10.83203125" style="2" customWidth="1"/>
+    <col min="16384" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="33" customHeight="1">
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="45" customHeight="1">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:8" s="5" customFormat="1" ht="17">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1">
+      <c r="A4" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1">
+      <c r="A5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="G8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="4"/>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
+    <row r="11" spans="1:8">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="H13" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="5" scale="68" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddFooter>&amp;LTab_43_rpt_PF_RecoveryForecast
 &amp;C&amp;P of &amp;N&amp;R{$date}</oddFooter>

</xml_diff>